<commit_message>
Major changes in Scoring Algorithm. Added TLD scores
</commit_message>
<xml_diff>
--- a/tests/test_data/test_emails.xlsx
+++ b/tests/test_data/test_emails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hawk007\PycharmProjects\PythonProject\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E137F4-4FB5-45AF-A7C2-732308092EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D963E6-3A27-4EB0-83AF-5E2C8411F276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Subject</t>
   </si>
@@ -139,16 +139,39 @@
   </si>
   <si>
     <t>A security breach originated from IP 91.218.114.25. Please reset your credentials immediately at the following link: http://bankofsecurity.org/validate-account</t>
+  </si>
+  <si>
+    <t>Visit this website and obtain your free gift.! : https://backoffice-dapp.vercel.app/filter-input</t>
+  </si>
+  <si>
+    <t>vercel.app@gifts.com</t>
+  </si>
+  <si>
+    <t>You have a gift.!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,13 +194,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +703,25 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{75D231DA-5602-48C8-9FBB-2785442F4623}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>